<commit_message>
update redis list for property
</commit_message>
<xml_diff>
--- a/onboarding-bootstrap/datav4.xlsx
+++ b/onboarding-bootstrap/datav4.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sachinkumarjha/bluemix-tutorials/microservices/hotels-onboarding-ui/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sachinkumarjha/bluemix-tutorials/microservices/1stSep/hotels-event-create/onboarding-bootstrap/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="24560" windowHeight="13560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hotels" sheetId="1" r:id="rId1"/>
     <sheet name="locations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="datafile" localSheetId="0">hotels!$A$1:$K$70</definedName>
-    <definedName name="hotels" localSheetId="0">hotels!$A$71:$K$111</definedName>
+    <definedName name="datafile" localSheetId="0">hotels!$A$1:$K$67</definedName>
+    <definedName name="hotels" localSheetId="0">hotels!$A$68:$K$108</definedName>
     <definedName name="locations" localSheetId="1">locations!$A$1:$J$10</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="523">
   <si>
     <t>placeid</t>
   </si>
@@ -1984,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2320,19 +2320,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -2347,24 +2347,24 @@
         <v>19</v>
       </c>
       <c r="J10">
-        <v>13.0556275</v>
+        <v>12.9489418</v>
       </c>
       <c r="K10">
-        <v>80.211094799999898</v>
+        <v>80.199946699999998</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -2382,27 +2382,27 @@
         <v>19</v>
       </c>
       <c r="J11">
-        <v>13.066016599999999</v>
+        <v>13.0485525</v>
       </c>
       <c r="K11">
-        <v>80.267217699999904</v>
+        <v>80.249810400000001</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -2417,27 +2417,27 @@
         <v>19</v>
       </c>
       <c r="J12">
-        <v>12.9489418</v>
+        <v>12.9699341</v>
       </c>
       <c r="K12">
-        <v>80.199946699999998</v>
+        <v>80.148457799999903</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -2452,24 +2452,24 @@
         <v>19</v>
       </c>
       <c r="J13">
-        <v>13.0485525</v>
+        <v>13.0710178</v>
       </c>
       <c r="K13">
-        <v>80.249810400000001</v>
+        <v>80.204853700000001</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -2487,27 +2487,27 @@
         <v>19</v>
       </c>
       <c r="J14">
-        <v>12.9699341</v>
+        <v>12.913874699999999</v>
       </c>
       <c r="K14">
-        <v>80.148457799999903</v>
+        <v>80.253179299999999</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -2522,30 +2522,30 @@
         <v>19</v>
       </c>
       <c r="J15">
-        <v>13.0710178</v>
+        <v>13.067765</v>
       </c>
       <c r="K15">
-        <v>80.204853700000001</v>
+        <v>80.259124700000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
@@ -2557,27 +2557,27 @@
         <v>19</v>
       </c>
       <c r="J16">
-        <v>12.913874699999999</v>
+        <v>13.036027199999999</v>
       </c>
       <c r="K16">
-        <v>80.253179299999999</v>
+        <v>80.145330699999903</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
@@ -2592,30 +2592,30 @@
         <v>19</v>
       </c>
       <c r="J17">
-        <v>13.067765</v>
+        <v>12.9733117</v>
       </c>
       <c r="K17">
-        <v>80.259124700000001</v>
+        <v>80.251001799999997</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
         <v>17</v>
@@ -2627,27 +2627,27 @@
         <v>19</v>
       </c>
       <c r="J18">
-        <v>13.036027199999999</v>
+        <v>12.9937389</v>
       </c>
       <c r="K18">
-        <v>80.145330699999903</v>
+        <v>80.186110399999905</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
         <v>16</v>
@@ -2662,24 +2662,24 @@
         <v>19</v>
       </c>
       <c r="J19">
-        <v>12.9733117</v>
+        <v>13.0658257</v>
       </c>
       <c r="K19">
-        <v>80.251001799999997</v>
+        <v>80.275670199999894</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -2697,24 +2697,24 @@
         <v>19</v>
       </c>
       <c r="J20">
-        <v>12.9937389</v>
+        <v>13.05334</v>
       </c>
       <c r="K20">
-        <v>80.186110399999905</v>
+        <v>80.268794999999898</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -2732,24 +2732,24 @@
         <v>19</v>
       </c>
       <c r="J21">
-        <v>13.0658257</v>
+        <v>13.070565</v>
       </c>
       <c r="K21">
-        <v>80.275670199999894</v>
+        <v>80.253285000000005</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -2767,24 +2767,24 @@
         <v>19</v>
       </c>
       <c r="J22">
-        <v>13.05334</v>
+        <v>12.99836</v>
       </c>
       <c r="K22">
-        <v>80.268794999999898</v>
+        <v>80.192961999999895</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -2802,24 +2802,24 @@
         <v>19</v>
       </c>
       <c r="J23">
-        <v>13.070565</v>
+        <v>13.027396899999999</v>
       </c>
       <c r="K23">
-        <v>80.253285000000005</v>
+        <v>80.253898199999895</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -2837,24 +2837,24 @@
         <v>19</v>
       </c>
       <c r="J24">
-        <v>12.99836</v>
+        <v>12.929088800000001</v>
       </c>
       <c r="K24">
-        <v>80.192961999999895</v>
+        <v>80.232832899999906</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2872,24 +2872,24 @@
         <v>19</v>
       </c>
       <c r="J25">
-        <v>13.027396899999999</v>
+        <v>13.0239998</v>
       </c>
       <c r="K25">
-        <v>80.253898199999895</v>
+        <v>80.201810300000005</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -2907,24 +2907,24 @@
         <v>19</v>
       </c>
       <c r="J26">
-        <v>12.929088800000001</v>
+        <v>13.053857000000001</v>
       </c>
       <c r="K26">
-        <v>80.232832899999906</v>
+        <v>80.240735299999898</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -2942,27 +2942,27 @@
         <v>19</v>
       </c>
       <c r="J27">
-        <v>13.0239998</v>
+        <v>12.989704400000001</v>
       </c>
       <c r="K27">
-        <v>80.201810300000005</v>
+        <v>80.260609199999905</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -2977,24 +2977,24 @@
         <v>19</v>
       </c>
       <c r="J28">
-        <v>13.053857000000001</v>
+        <v>13.0525366</v>
       </c>
       <c r="K28">
-        <v>80.240735299999898</v>
+        <v>80.235609599999904</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D29" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
@@ -3012,27 +3012,27 @@
         <v>19</v>
       </c>
       <c r="J29">
-        <v>13.053857000000001</v>
+        <v>13.1170613</v>
       </c>
       <c r="K29">
-        <v>80.240735299999898</v>
+        <v>80.284253399999997</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -3047,27 +3047,27 @@
         <v>19</v>
       </c>
       <c r="J30">
-        <v>12.989704400000001</v>
+        <v>12.9893786</v>
       </c>
       <c r="K30">
-        <v>80.260609199999905</v>
+        <v>80.2208854</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -3082,24 +3082,24 @@
         <v>19</v>
       </c>
       <c r="J31">
-        <v>13.0525366</v>
+        <v>13.065486</v>
       </c>
       <c r="K31">
-        <v>80.235609599999904</v>
+        <v>80.210329999999999</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -3117,27 +3117,27 @@
         <v>19</v>
       </c>
       <c r="J32">
-        <v>13.1170613</v>
+        <v>13.052911</v>
       </c>
       <c r="K32">
-        <v>80.284253399999997</v>
+        <v>80.248334999999997</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -3152,24 +3152,24 @@
         <v>19</v>
       </c>
       <c r="J33">
-        <v>12.9893786</v>
+        <v>13.066573200000001</v>
       </c>
       <c r="K33">
-        <v>80.2208854</v>
+        <v>80.273984199999902</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -3187,27 +3187,27 @@
         <v>19</v>
       </c>
       <c r="J34">
-        <v>13.065486</v>
+        <v>13.080573299999999</v>
       </c>
       <c r="K34">
-        <v>80.210329999999999</v>
+        <v>80.2674489999999</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
         <v>16</v>
@@ -3222,27 +3222,27 @@
         <v>19</v>
       </c>
       <c r="J35">
-        <v>13.052911</v>
+        <v>13.040408100000001</v>
       </c>
       <c r="K35">
-        <v>80.248334999999997</v>
+        <v>80.243798900000002</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F36" t="s">
         <v>16</v>
@@ -3257,27 +3257,27 @@
         <v>19</v>
       </c>
       <c r="J36">
-        <v>13.066573200000001</v>
+        <v>13.0453803</v>
       </c>
       <c r="K36">
-        <v>80.273984199999902</v>
+        <v>80.232196700000003</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
@@ -3292,27 +3292,27 @@
         <v>19</v>
       </c>
       <c r="J37">
-        <v>13.080573299999999</v>
+        <v>13.028941</v>
       </c>
       <c r="K37">
-        <v>80.2674489999999</v>
+        <v>80.2524599999999</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="F38" t="s">
         <v>16</v>
@@ -3327,27 +3327,27 @@
         <v>19</v>
       </c>
       <c r="J38">
-        <v>13.040408100000001</v>
+        <v>13.0286443</v>
       </c>
       <c r="K38">
-        <v>80.243798900000002</v>
+        <v>80.252726999999993</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C39" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="F39" t="s">
         <v>16</v>
@@ -3362,27 +3362,27 @@
         <v>19</v>
       </c>
       <c r="J39">
-        <v>13.0453803</v>
+        <v>13.079223499999999</v>
       </c>
       <c r="K39">
-        <v>80.232196700000003</v>
+        <v>80.249297200000001</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E40" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
         <v>16</v>
@@ -3397,27 +3397,27 @@
         <v>19</v>
       </c>
       <c r="J40">
-        <v>13.028941</v>
+        <v>13.052883</v>
       </c>
       <c r="K40">
-        <v>80.2524599999999</v>
+        <v>80.2498594999999</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="E41" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="F41" t="s">
         <v>16</v>
@@ -3432,27 +3432,27 @@
         <v>19</v>
       </c>
       <c r="J41">
-        <v>13.0286443</v>
+        <v>12.998633</v>
       </c>
       <c r="K41">
-        <v>80.252726999999993</v>
+        <v>80.192794999999904</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D42" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="E42" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="F42" t="s">
         <v>16</v>
@@ -3467,27 +3467,27 @@
         <v>19</v>
       </c>
       <c r="J42">
-        <v>13.079223499999999</v>
+        <v>13.0341922</v>
       </c>
       <c r="K42">
-        <v>80.249297200000001</v>
+        <v>80.235831200000007</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C43" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
       <c r="F43" t="s">
         <v>16</v>
@@ -3502,24 +3502,24 @@
         <v>19</v>
       </c>
       <c r="J43">
-        <v>13.052883</v>
+        <v>13.066647</v>
       </c>
       <c r="K43">
-        <v>80.2498594999999</v>
+        <v>80.270111999999898</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="C44" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D44" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
@@ -3537,24 +3537,24 @@
         <v>19</v>
       </c>
       <c r="J44">
-        <v>12.998633</v>
+        <v>13.017989</v>
       </c>
       <c r="K44">
-        <v>80.192794999999904</v>
+        <v>80.272654500000002</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C45" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="D45" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -3572,27 +3572,27 @@
         <v>19</v>
       </c>
       <c r="J45">
-        <v>13.0341922</v>
+        <v>13.072527300000001</v>
       </c>
       <c r="K45">
-        <v>80.235831200000007</v>
+        <v>80.2548587</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="E46" t="s">
-        <v>199</v>
+        <v>16</v>
       </c>
       <c r="F46" t="s">
         <v>16</v>
@@ -3607,24 +3607,24 @@
         <v>19</v>
       </c>
       <c r="J46">
-        <v>13.066647</v>
+        <v>13.039363</v>
       </c>
       <c r="K46">
-        <v>80.270111999999898</v>
+        <v>80.244801999999893</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="D47" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
@@ -3642,27 +3642,27 @@
         <v>19</v>
       </c>
       <c r="J47">
-        <v>13.017989</v>
+        <v>12.905556000000001</v>
       </c>
       <c r="K47">
-        <v>80.272654500000002</v>
+        <v>80.227624999999904</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B48" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="D48" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="F48" t="s">
         <v>16</v>
@@ -3677,27 +3677,27 @@
         <v>19</v>
       </c>
       <c r="J48">
-        <v>13.072527300000001</v>
+        <v>13.014215800000001</v>
       </c>
       <c r="K48">
-        <v>80.2548587</v>
+        <v>80.222803699999901</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="C49" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="D49" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="E49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F49" t="s">
         <v>16</v>
@@ -3712,27 +3712,27 @@
         <v>19</v>
       </c>
       <c r="J49">
-        <v>13.039363</v>
+        <v>13.051738500000001</v>
       </c>
       <c r="K49">
-        <v>80.244801999999893</v>
+        <v>80.240448599999993</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C50" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="D50" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
+        <v>229</v>
       </c>
       <c r="F50" t="s">
         <v>16</v>
@@ -3747,30 +3747,30 @@
         <v>19</v>
       </c>
       <c r="J50">
-        <v>12.905556000000001</v>
+        <v>13.029421899999999</v>
       </c>
       <c r="K50">
-        <v>80.227624999999904</v>
+        <v>80.245448300000007</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C51" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="D51" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="E51" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="G51" t="s">
         <v>17</v>
@@ -3782,27 +3782,27 @@
         <v>19</v>
       </c>
       <c r="J51">
-        <v>13.014215800000001</v>
+        <v>12.910631</v>
       </c>
       <c r="K51">
-        <v>80.222803699999901</v>
+        <v>80.228671999999904</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="D52" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="E52" t="s">
-        <v>15</v>
+        <v>239</v>
       </c>
       <c r="F52" t="s">
         <v>16</v>
@@ -3817,27 +3817,27 @@
         <v>19</v>
       </c>
       <c r="J52">
-        <v>13.051738500000001</v>
+        <v>13.0671167</v>
       </c>
       <c r="K52">
-        <v>80.240448599999993</v>
+        <v>80.258163999999894</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="B53" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="C53" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="D53" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="E53" t="s">
-        <v>229</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
         <v>16</v>
@@ -3852,30 +3852,30 @@
         <v>19</v>
       </c>
       <c r="J53">
-        <v>13.029421899999999</v>
+        <v>13.065225</v>
       </c>
       <c r="K53">
-        <v>80.245448300000007</v>
+        <v>80.240197999999907</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B54" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="C54" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="D54" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>234</v>
+        <v>16</v>
       </c>
       <c r="G54" t="s">
         <v>17</v>
@@ -3887,27 +3887,27 @@
         <v>19</v>
       </c>
       <c r="J54">
-        <v>12.910631</v>
+        <v>13.0625061</v>
       </c>
       <c r="K54">
-        <v>80.228671999999904</v>
+        <v>80.274074799999994</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="B55" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="C55" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="D55" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="E55" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
@@ -3922,27 +3922,27 @@
         <v>19</v>
       </c>
       <c r="J55">
-        <v>13.0671167</v>
+        <v>13.0636916</v>
       </c>
       <c r="K55">
-        <v>80.258163999999894</v>
+        <v>80.277673899999897</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="B56" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="C56" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="D56" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
@@ -3957,24 +3957,24 @@
         <v>19</v>
       </c>
       <c r="J56">
-        <v>13.065225</v>
+        <v>13.0392771</v>
       </c>
       <c r="K56">
-        <v>80.240197999999907</v>
+        <v>80.229311699999897</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="B57" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="C57" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="D57" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -3992,27 +3992,27 @@
         <v>19</v>
       </c>
       <c r="J57">
-        <v>13.0625061</v>
+        <v>13.058249099999999</v>
       </c>
       <c r="K57">
-        <v>80.274074799999994</v>
+        <v>80.247637599999905</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C58" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="D58" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="E58" t="s">
-        <v>252</v>
+        <v>15</v>
       </c>
       <c r="F58" t="s">
         <v>16</v>
@@ -4027,27 +4027,27 @@
         <v>19</v>
       </c>
       <c r="J58">
-        <v>13.0636916</v>
+        <v>13.061400900000001</v>
       </c>
       <c r="K58">
-        <v>80.277673899999897</v>
+        <v>80.263891599999894</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B59" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C59" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D59" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="E59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F59" t="s">
         <v>16</v>
@@ -4062,24 +4062,24 @@
         <v>19</v>
       </c>
       <c r="J59">
-        <v>13.0392771</v>
+        <v>13.04139</v>
       </c>
       <c r="K59">
-        <v>80.229311699999897</v>
+        <v>80.234351999999902</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C60" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="D60" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -4097,27 +4097,27 @@
         <v>19</v>
       </c>
       <c r="J60">
-        <v>13.058249099999999</v>
+        <v>13.04139</v>
       </c>
       <c r="K60">
-        <v>80.247637599999905</v>
+        <v>80.234351999999902</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B61" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="C61" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="D61" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E61" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F61" t="s">
         <v>16</v>
@@ -4132,30 +4132,30 @@
         <v>19</v>
       </c>
       <c r="J61">
-        <v>13.061400900000001</v>
+        <v>13.0429815</v>
       </c>
       <c r="K61">
-        <v>80.263891599999894</v>
+        <v>80.230713100000003</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="B62" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C62" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="D62" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E62" t="s">
-        <v>15</v>
+        <v>277</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
+        <v>278</v>
       </c>
       <c r="G62" t="s">
         <v>17</v>
@@ -4167,24 +4167,24 @@
         <v>19</v>
       </c>
       <c r="J62">
-        <v>13.04139</v>
+        <v>12.786357799999999</v>
       </c>
       <c r="K62">
-        <v>80.234351999999902</v>
+        <v>80.221242099999898</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B63" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="C63" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="D63" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -4202,27 +4202,27 @@
         <v>19</v>
       </c>
       <c r="J63">
-        <v>13.04139</v>
+        <v>13.0398233</v>
       </c>
       <c r="K63">
-        <v>80.234351999999902</v>
+        <v>80.2343683</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="B64" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="C64" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="D64" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="E64" t="s">
-        <v>136</v>
+        <v>287</v>
       </c>
       <c r="F64" t="s">
         <v>16</v>
@@ -4237,30 +4237,30 @@
         <v>19</v>
       </c>
       <c r="J64">
-        <v>13.0429815</v>
+        <v>13.0859211</v>
       </c>
       <c r="K64">
-        <v>80.230713100000003</v>
+        <v>80.223270200000002</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B65" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C65" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="D65" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="E65" t="s">
-        <v>277</v>
+        <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
       <c r="G65" t="s">
         <v>17</v>
@@ -4272,24 +4272,24 @@
         <v>19</v>
       </c>
       <c r="J65">
-        <v>12.786357799999999</v>
+        <v>13.0495286</v>
       </c>
       <c r="K65">
-        <v>80.221242099999898</v>
+        <v>80.249609999999905</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="B66" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C66" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="D66" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -4307,27 +4307,27 @@
         <v>19</v>
       </c>
       <c r="J66">
-        <v>13.0398233</v>
+        <v>13.017277999999999</v>
       </c>
       <c r="K66">
-        <v>80.2343683</v>
+        <v>80.270637999999906</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="B67" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="C67" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="D67" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="E67" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="F67" t="s">
         <v>16</v>
@@ -4342,24 +4342,24 @@
         <v>19</v>
       </c>
       <c r="J67">
-        <v>13.0859211</v>
+        <v>13.0355676</v>
       </c>
       <c r="K67">
-        <v>80.223270200000002</v>
+        <v>80.238733999999994</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B68" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C68" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D68" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -4377,24 +4377,24 @@
         <v>19</v>
       </c>
       <c r="J68">
-        <v>13.0495286</v>
+        <v>12.8996002</v>
       </c>
       <c r="K68">
-        <v>80.249609999999905</v>
+        <v>80.228813799999998</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>292</v>
+        <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>293</v>
+        <v>50</v>
       </c>
       <c r="C69" t="s">
-        <v>294</v>
+        <v>51</v>
       </c>
       <c r="D69" t="s">
-        <v>295</v>
+        <v>52</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -4412,27 +4412,27 @@
         <v>19</v>
       </c>
       <c r="J69">
-        <v>13.017277999999999</v>
+        <v>13.0556275</v>
       </c>
       <c r="K69">
-        <v>80.270637999999906</v>
+        <v>80.211094799999898</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>296</v>
+        <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>297</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>298</v>
+        <v>55</v>
       </c>
       <c r="D70" t="s">
-        <v>299</v>
+        <v>56</v>
       </c>
       <c r="E70" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F70" t="s">
         <v>16</v>
@@ -4447,24 +4447,24 @@
         <v>19</v>
       </c>
       <c r="J70">
-        <v>13.0355676</v>
+        <v>13.066016599999999</v>
       </c>
       <c r="K70">
-        <v>80.238733999999994</v>
+        <v>80.267217699999904</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B71" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C71" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D71" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -4482,27 +4482,27 @@
         <v>19</v>
       </c>
       <c r="J71">
-        <v>12.8996002</v>
+        <v>13.042828699999999</v>
       </c>
       <c r="K71">
-        <v>80.228813799999998</v>
+        <v>80.261150899999905</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>49</v>
+        <v>308</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>309</v>
       </c>
       <c r="C72" t="s">
-        <v>51</v>
+        <v>310</v>
       </c>
       <c r="D72" t="s">
-        <v>52</v>
+        <v>311</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
       <c r="F72" t="s">
         <v>16</v>
@@ -4517,27 +4517,27 @@
         <v>19</v>
       </c>
       <c r="J72">
-        <v>13.0556275</v>
+        <v>13.009577699999999</v>
       </c>
       <c r="K72">
-        <v>80.211094799999898</v>
+        <v>80.250277499999996</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>53</v>
+        <v>313</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>55</v>
+        <v>315</v>
       </c>
       <c r="D73" t="s">
-        <v>56</v>
+        <v>316</v>
       </c>
       <c r="E73" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
@@ -4552,24 +4552,24 @@
         <v>19</v>
       </c>
       <c r="J73">
-        <v>13.066016599999999</v>
+        <v>13.0323814</v>
       </c>
       <c r="K73">
-        <v>80.267217699999904</v>
+        <v>80.232834499999896</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="B74" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="C74" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="D74" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
@@ -4587,27 +4587,27 @@
         <v>19</v>
       </c>
       <c r="J74">
-        <v>13.042828699999999</v>
+        <v>13.0659551</v>
       </c>
       <c r="K74">
-        <v>80.261150899999905</v>
+        <v>80.275071999999994</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="B75" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="C75" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="D75" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="E75" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
@@ -4622,27 +4622,27 @@
         <v>19</v>
       </c>
       <c r="J75">
-        <v>13.009577699999999</v>
+        <v>13.068490300000001</v>
       </c>
       <c r="K75">
-        <v>80.250277499999996</v>
+        <v>80.194793699999906</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="B76" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="C76" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="D76" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="E76" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
@@ -4657,27 +4657,27 @@
         <v>19</v>
       </c>
       <c r="J76">
-        <v>13.0323814</v>
+        <v>12.983451799999999</v>
       </c>
       <c r="K76">
-        <v>80.232834499999896</v>
+        <v>80.2462952999999</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="B77" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="C77" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="D77" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="E77" t="s">
-        <v>15</v>
+        <v>334</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -4692,27 +4692,27 @@
         <v>19</v>
       </c>
       <c r="J77">
-        <v>13.0659551</v>
+        <v>13.0638448</v>
       </c>
       <c r="K77">
-        <v>80.275071999999994</v>
+        <v>80.210179199999899</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="B78" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="C78" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="D78" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="E78" t="s">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -4727,27 +4727,27 @@
         <v>19</v>
       </c>
       <c r="J78">
-        <v>13.068490300000001</v>
+        <v>12.9662223</v>
       </c>
       <c r="K78">
-        <v>80.194793699999906</v>
+        <v>80.149137999999994</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="B79" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C79" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D79" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="E79" t="s">
-        <v>15</v>
+        <v>343</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -4762,27 +4762,27 @@
         <v>19</v>
       </c>
       <c r="J79">
-        <v>12.983451799999999</v>
+        <v>12.9700638</v>
       </c>
       <c r="K79">
-        <v>80.2462952999999</v>
+        <v>80.1460521999999</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="B80" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="C80" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="D80" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="E80" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
@@ -4797,24 +4797,24 @@
         <v>19</v>
       </c>
       <c r="J80">
-        <v>13.0638448</v>
+        <v>13.071020000000001</v>
       </c>
       <c r="K80">
-        <v>80.210179199999899</v>
+        <v>80.211237999999895</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="B81" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="C81" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D81" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -4832,27 +4832,27 @@
         <v>19</v>
       </c>
       <c r="J81">
-        <v>12.9662223</v>
+        <v>13.0805325</v>
       </c>
       <c r="K81">
-        <v>80.149137999999994</v>
+        <v>80.269378899999893</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="B82" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="C82" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="D82" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="E82" t="s">
-        <v>343</v>
+        <v>15</v>
       </c>
       <c r="F82" t="s">
         <v>16</v>
@@ -4867,27 +4867,27 @@
         <v>19</v>
       </c>
       <c r="J82">
-        <v>12.9700638</v>
+        <v>13.0460004</v>
       </c>
       <c r="K82">
-        <v>80.1460521999999</v>
+        <v>80.239401199999904</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="B83" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="C83" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="D83" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="E83" t="s">
-        <v>348</v>
+        <v>15</v>
       </c>
       <c r="F83" t="s">
         <v>16</v>
@@ -4902,24 +4902,24 @@
         <v>19</v>
       </c>
       <c r="J83">
-        <v>13.071020000000001</v>
+        <v>13.078876299999999</v>
       </c>
       <c r="K83">
-        <v>80.211237999999895</v>
+        <v>80.241307599999999</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B84" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="C84" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="D84" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -4937,24 +4937,24 @@
         <v>19</v>
       </c>
       <c r="J84">
-        <v>13.0805325</v>
+        <v>13.052080800000001</v>
       </c>
       <c r="K84">
-        <v>80.269378899999893</v>
+        <v>80.212246800000003</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="B85" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
       <c r="C85" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="D85" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -4972,27 +4972,27 @@
         <v>19</v>
       </c>
       <c r="J85">
-        <v>13.0460004</v>
+        <v>13.0385641</v>
       </c>
       <c r="K85">
-        <v>80.239401199999904</v>
+        <v>80.232291000000004</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="B86" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="C86" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="D86" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="E86" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F86" t="s">
         <v>16</v>
@@ -5007,24 +5007,24 @@
         <v>19</v>
       </c>
       <c r="J86">
-        <v>13.078876299999999</v>
+        <v>13.037652</v>
       </c>
       <c r="K86">
-        <v>80.241307599999999</v>
+        <v>80.231413999999901</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="B87" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="C87" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="D87" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -5036,30 +5036,30 @@
         <v>17</v>
       </c>
       <c r="H87" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="I87" t="s">
         <v>19</v>
       </c>
       <c r="J87">
-        <v>13.052080800000001</v>
+        <v>13.0447028</v>
       </c>
       <c r="K87">
-        <v>80.212246800000003</v>
+        <v>80.242254699999904</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="B88" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="C88" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D88" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -5077,27 +5077,27 @@
         <v>19</v>
       </c>
       <c r="J88">
-        <v>13.0385641</v>
+        <v>13.0468963</v>
       </c>
       <c r="K88">
-        <v>80.232291000000004</v>
+        <v>80.218684599999904</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="B89" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="C89" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="D89" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="E89" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F89" t="s">
         <v>16</v>
@@ -5112,27 +5112,27 @@
         <v>19</v>
       </c>
       <c r="J89">
-        <v>13.037652</v>
+        <v>12.959902899999999</v>
       </c>
       <c r="K89">
-        <v>80.231413999999901</v>
+        <v>80.143556199999907</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="B90" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="C90" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="D90" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="E90" t="s">
-        <v>15</v>
+        <v>239</v>
       </c>
       <c r="F90" t="s">
         <v>16</v>
@@ -5141,33 +5141,33 @@
         <v>17</v>
       </c>
       <c r="H90" t="s">
-        <v>377</v>
+        <v>18</v>
       </c>
       <c r="I90" t="s">
         <v>19</v>
       </c>
       <c r="J90">
-        <v>13.0447028</v>
+        <v>13.077416100000001</v>
       </c>
       <c r="K90">
-        <v>80.242254699999904</v>
+        <v>80.2625124999999</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="B91" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="C91" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D91" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="E91" t="s">
-        <v>15</v>
+        <v>394</v>
       </c>
       <c r="F91" t="s">
         <v>16</v>
@@ -5182,24 +5182,24 @@
         <v>19</v>
       </c>
       <c r="J91">
-        <v>13.0468963</v>
+        <v>13.0951121</v>
       </c>
       <c r="K91">
-        <v>80.218684599999904</v>
+        <v>80.290615099999897</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="B92" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="C92" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="D92" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -5217,27 +5217,27 @@
         <v>19</v>
       </c>
       <c r="J92">
-        <v>12.959902899999999</v>
+        <v>13.043789500000001</v>
       </c>
       <c r="K92">
-        <v>80.143556199999907</v>
+        <v>80.2711501</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="B93" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="C93" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="D93" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="E93" t="s">
-        <v>239</v>
+        <v>403</v>
       </c>
       <c r="F93" t="s">
         <v>16</v>
@@ -5252,27 +5252,27 @@
         <v>19</v>
       </c>
       <c r="J93">
-        <v>13.077416100000001</v>
+        <v>13.0389211</v>
       </c>
       <c r="K93">
-        <v>80.2625124999999</v>
+        <v>80.259598199999999</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="B94" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="C94" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="D94" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="E94" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="F94" t="s">
         <v>16</v>
@@ -5287,27 +5287,27 @@
         <v>19</v>
       </c>
       <c r="J94">
-        <v>13.0951121</v>
+        <v>13.045895</v>
       </c>
       <c r="K94">
-        <v>80.290615099999897</v>
+        <v>80.247795999999994</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="B95" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="C95" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="D95" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="E95" t="s">
-        <v>15</v>
+        <v>413</v>
       </c>
       <c r="F95" t="s">
         <v>16</v>
@@ -5322,27 +5322,27 @@
         <v>19</v>
       </c>
       <c r="J95">
-        <v>13.043789500000001</v>
+        <v>13.064401500000001</v>
       </c>
       <c r="K95">
-        <v>80.2711501</v>
+        <v>80.243316300000004</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>399</v>
+        <v>414</v>
       </c>
       <c r="B96" t="s">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="C96" t="s">
-        <v>401</v>
+        <v>416</v>
       </c>
       <c r="D96" t="s">
-        <v>402</v>
+        <v>417</v>
       </c>
       <c r="E96" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="F96" t="s">
         <v>16</v>
@@ -5357,27 +5357,27 @@
         <v>19</v>
       </c>
       <c r="J96">
-        <v>13.0389211</v>
+        <v>13.064094600000001</v>
       </c>
       <c r="K96">
-        <v>80.259598199999999</v>
+        <v>80.242161600000003</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="B97" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="C97" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="D97" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="E97" t="s">
-        <v>408</v>
+        <v>15</v>
       </c>
       <c r="F97" t="s">
         <v>16</v>
@@ -5392,27 +5392,27 @@
         <v>19</v>
       </c>
       <c r="J97">
-        <v>13.045895</v>
+        <v>13.0542792</v>
       </c>
       <c r="K97">
-        <v>80.247795999999994</v>
+        <v>80.253177499999893</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="B98" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="C98" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="D98" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="E98" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="F98" t="s">
         <v>16</v>
@@ -5427,27 +5427,27 @@
         <v>19</v>
       </c>
       <c r="J98">
-        <v>13.064401500000001</v>
+        <v>13.046714100000001</v>
       </c>
       <c r="K98">
-        <v>80.243316300000004</v>
+        <v>80.266620900000007</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="B99" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="C99" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="D99" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="E99" t="s">
-        <v>413</v>
+        <v>136</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
@@ -5462,27 +5462,27 @@
         <v>19</v>
       </c>
       <c r="J99">
-        <v>13.064094600000001</v>
+        <v>13.044298</v>
       </c>
       <c r="K99">
-        <v>80.242161600000003</v>
+        <v>80.238319699999906</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="B100" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="C100" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="D100" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="E100" t="s">
-        <v>15</v>
+        <v>434</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
@@ -5497,27 +5497,27 @@
         <v>19</v>
       </c>
       <c r="J100">
-        <v>13.0542792</v>
+        <v>13.045194</v>
       </c>
       <c r="K100">
-        <v>80.253177499999893</v>
+        <v>80.189204000000004</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="B101" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="C101" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="D101" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="E101" t="s">
-        <v>403</v>
+        <v>15</v>
       </c>
       <c r="F101" t="s">
         <v>16</v>
@@ -5532,27 +5532,27 @@
         <v>19</v>
       </c>
       <c r="J101">
-        <v>13.046714100000001</v>
+        <v>13.05884</v>
       </c>
       <c r="K101">
-        <v>80.266620900000007</v>
+        <v>80.263026999999894</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="B102" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="C102" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="D102" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="E102" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F102" t="s">
         <v>16</v>
@@ -5567,30 +5567,30 @@
         <v>19</v>
       </c>
       <c r="J102">
-        <v>13.044298</v>
+        <v>13.038558999999999</v>
       </c>
       <c r="K102">
-        <v>80.238319699999906</v>
+        <v>80.258137000000005</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="B103" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="C103" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="D103" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="E103" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="F103" t="s">
-        <v>16</v>
+        <v>448</v>
       </c>
       <c r="G103" t="s">
         <v>17</v>
@@ -5602,27 +5602,27 @@
         <v>19</v>
       </c>
       <c r="J103">
-        <v>13.045194</v>
+        <v>12.844614699999999</v>
       </c>
       <c r="K103">
-        <v>80.189204000000004</v>
+        <v>80.243062699999996</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="B104" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C104" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="D104" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E104" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -5637,24 +5637,24 @@
         <v>19</v>
       </c>
       <c r="J104">
-        <v>13.05884</v>
+        <v>13.038517300000001</v>
       </c>
       <c r="K104">
-        <v>80.263026999999894</v>
+        <v>80.239962599999998</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="B105" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="C105" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="D105" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -5672,30 +5672,30 @@
         <v>19</v>
       </c>
       <c r="J105">
-        <v>13.038558999999999</v>
+        <v>13.0867883</v>
       </c>
       <c r="K105">
-        <v>80.258137000000005</v>
+        <v>80.269808900000001</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>443</v>
+        <v>457</v>
       </c>
       <c r="B106" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C106" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="D106" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="E106" t="s">
-        <v>447</v>
+        <v>15</v>
       </c>
       <c r="F106" t="s">
-        <v>448</v>
+        <v>16</v>
       </c>
       <c r="G106" t="s">
         <v>17</v>
@@ -5707,24 +5707,24 @@
         <v>19</v>
       </c>
       <c r="J106">
-        <v>12.844614699999999</v>
+        <v>13.067836</v>
       </c>
       <c r="K106">
-        <v>80.243062699999996</v>
+        <v>80.271991999999898</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B107" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C107" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="D107" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="E107" t="s">
         <v>136</v>
@@ -5742,30 +5742,30 @@
         <v>19</v>
       </c>
       <c r="J107">
-        <v>13.038517300000001</v>
+        <v>13.050005000000001</v>
       </c>
       <c r="K107">
-        <v>80.239962599999998</v>
+        <v>80.232989999999901</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B108" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="C108" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="D108" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="E108" t="s">
         <v>15</v>
       </c>
       <c r="F108" t="s">
-        <v>16</v>
+        <v>469</v>
       </c>
       <c r="G108" t="s">
         <v>17</v>
@@ -5777,114 +5777,9 @@
         <v>19</v>
       </c>
       <c r="J108">
-        <v>13.0867883</v>
+        <v>12.764486</v>
       </c>
       <c r="K108">
-        <v>80.269808900000001</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="B109" t="s">
-        <v>458</v>
-      </c>
-      <c r="C109" t="s">
-        <v>459</v>
-      </c>
-      <c r="D109" t="s">
-        <v>460</v>
-      </c>
-      <c r="E109" t="s">
-        <v>15</v>
-      </c>
-      <c r="F109" t="s">
-        <v>16</v>
-      </c>
-      <c r="G109" t="s">
-        <v>17</v>
-      </c>
-      <c r="H109" t="s">
-        <v>18</v>
-      </c>
-      <c r="I109" t="s">
-        <v>19</v>
-      </c>
-      <c r="J109">
-        <v>13.067836</v>
-      </c>
-      <c r="K109">
-        <v>80.271991999999898</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="B110" t="s">
-        <v>462</v>
-      </c>
-      <c r="C110" t="s">
-        <v>463</v>
-      </c>
-      <c r="D110" t="s">
-        <v>464</v>
-      </c>
-      <c r="E110" t="s">
-        <v>136</v>
-      </c>
-      <c r="F110" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" t="s">
-        <v>17</v>
-      </c>
-      <c r="H110" t="s">
-        <v>18</v>
-      </c>
-      <c r="I110" t="s">
-        <v>19</v>
-      </c>
-      <c r="J110">
-        <v>13.050005000000001</v>
-      </c>
-      <c r="K110">
-        <v>80.232989999999901</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B111" t="s">
-        <v>466</v>
-      </c>
-      <c r="C111" t="s">
-        <v>467</v>
-      </c>
-      <c r="D111" t="s">
-        <v>468</v>
-      </c>
-      <c r="E111" t="s">
-        <v>15</v>
-      </c>
-      <c r="F111" t="s">
-        <v>469</v>
-      </c>
-      <c r="G111" t="s">
-        <v>17</v>
-      </c>
-      <c r="H111" t="s">
-        <v>18</v>
-      </c>
-      <c r="I111" t="s">
-        <v>19</v>
-      </c>
-      <c r="J111">
-        <v>12.764486</v>
-      </c>
-      <c r="K111">
         <v>80.005634999999899</v>
       </c>
     </row>
@@ -5897,7 +5792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
remove duplicate entries from bootstrap file
</commit_message>
<xml_diff>
--- a/onboarding-bootstrap/datav4.xlsx
+++ b/onboarding-bootstrap/datav4.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hotels" sheetId="1" r:id="rId1"/>
     <sheet name="locations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="datafile" localSheetId="0">hotels!$A$1:$K$67</definedName>
-    <definedName name="hotels" localSheetId="0">hotels!$A$68:$K$108</definedName>
+    <definedName name="datafile" localSheetId="0">hotels!$A$1:$K$66</definedName>
+    <definedName name="hotels" localSheetId="0">hotels!$A$67:$K$107</definedName>
     <definedName name="locations" localSheetId="1">locations!$A$1:$J$10</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -35,7 +35,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="datafile" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sachinkumarjha/bluemix-tutorials/microservices/hotels-onboarding-ui/datafile.csv" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/sachinkumarjha/bluemix-tutorials/microservices/hotels-onboarding-ui/datafile.csv" semicolon="1">
       <textFields count="11">
         <textField type="text"/>
         <textField/>
@@ -52,7 +52,7 @@
     </textPr>
   </connection>
   <connection id="2" name="hotels" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sachinkumarjha/Documents/SametimeFileTransfers/hotels.csv" tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/sachinkumarjha/Documents/SametimeFileTransfers/hotels.csv" tab="0" semicolon="1">
       <textFields count="11">
         <textField type="text"/>
         <textField/>
@@ -69,7 +69,7 @@
     </textPr>
   </connection>
   <connection id="3" name="locations" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/sachinkumarjha/bluemix-tutorials/microservices/hotels-onboarding-ui/locations.csv" tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/sachinkumarjha/bluemix-tutorials/microservices/hotels-onboarding-ui/locations.csv" tab="0" semicolon="1">
       <textFields count="10">
         <textField type="text"/>
         <textField/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="523">
   <si>
     <t>placeid</t>
   </si>
@@ -1984,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4070,19 +4070,19 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B60" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C60" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D60" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F60" t="s">
         <v>16</v>
@@ -4097,30 +4097,30 @@
         <v>19</v>
       </c>
       <c r="J60">
-        <v>13.04139</v>
+        <v>13.0429815</v>
       </c>
       <c r="K60">
-        <v>80.234351999999902</v>
+        <v>80.230713100000003</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B61" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C61" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D61" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E61" t="s">
-        <v>136</v>
+        <v>277</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>278</v>
       </c>
       <c r="G61" t="s">
         <v>17</v>
@@ -4132,30 +4132,30 @@
         <v>19</v>
       </c>
       <c r="J61">
-        <v>13.0429815</v>
+        <v>12.786357799999999</v>
       </c>
       <c r="K61">
-        <v>80.230713100000003</v>
+        <v>80.221242099999898</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B62" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C62" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D62" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E62" t="s">
-        <v>277</v>
+        <v>15</v>
       </c>
       <c r="F62" t="s">
-        <v>278</v>
+        <v>16</v>
       </c>
       <c r="G62" t="s">
         <v>17</v>
@@ -4167,27 +4167,27 @@
         <v>19</v>
       </c>
       <c r="J62">
-        <v>12.786357799999999</v>
+        <v>13.0398233</v>
       </c>
       <c r="K62">
-        <v>80.221242099999898</v>
+        <v>80.2343683</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B63" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C63" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D63" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E63" t="s">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="F63" t="s">
         <v>16</v>
@@ -4202,27 +4202,27 @@
         <v>19</v>
       </c>
       <c r="J63">
-        <v>13.0398233</v>
+        <v>13.0859211</v>
       </c>
       <c r="K63">
-        <v>80.2343683</v>
+        <v>80.223270200000002</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B64" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C64" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D64" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="E64" t="s">
-        <v>287</v>
+        <v>15</v>
       </c>
       <c r="F64" t="s">
         <v>16</v>
@@ -4237,24 +4237,24 @@
         <v>19</v>
       </c>
       <c r="J64">
-        <v>13.0859211</v>
+        <v>13.0495286</v>
       </c>
       <c r="K64">
-        <v>80.223270200000002</v>
+        <v>80.249609999999905</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B65" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C65" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D65" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -4272,27 +4272,27 @@
         <v>19</v>
       </c>
       <c r="J65">
-        <v>13.0495286</v>
+        <v>13.017277999999999</v>
       </c>
       <c r="K65">
-        <v>80.249609999999905</v>
+        <v>80.270637999999906</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B66" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C66" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D66" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E66" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F66" t="s">
         <v>16</v>
@@ -4307,27 +4307,27 @@
         <v>19</v>
       </c>
       <c r="J66">
-        <v>13.017277999999999</v>
+        <v>13.0355676</v>
       </c>
       <c r="K66">
-        <v>80.270637999999906</v>
+        <v>80.238733999999994</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B67" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C67" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D67" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="E67" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F67" t="s">
         <v>16</v>
@@ -4342,24 +4342,24 @@
         <v>19</v>
       </c>
       <c r="J67">
-        <v>13.0355676</v>
+        <v>12.8996002</v>
       </c>
       <c r="K67">
-        <v>80.238733999999994</v>
+        <v>80.228813799999998</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>300</v>
+        <v>49</v>
       </c>
       <c r="B68" t="s">
-        <v>301</v>
+        <v>50</v>
       </c>
       <c r="C68" t="s">
-        <v>302</v>
+        <v>51</v>
       </c>
       <c r="D68" t="s">
-        <v>303</v>
+        <v>52</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -4377,24 +4377,24 @@
         <v>19</v>
       </c>
       <c r="J68">
-        <v>12.8996002</v>
+        <v>13.0556275</v>
       </c>
       <c r="K68">
-        <v>80.228813799999998</v>
+        <v>80.211094799999898</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -4412,24 +4412,24 @@
         <v>19</v>
       </c>
       <c r="J69">
-        <v>13.0556275</v>
+        <v>13.066016599999999</v>
       </c>
       <c r="K69">
-        <v>80.211094799999898</v>
+        <v>80.267217699999904</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>53</v>
+        <v>304</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>305</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>306</v>
       </c>
       <c r="D70" t="s">
-        <v>56</v>
+        <v>307</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -4447,27 +4447,27 @@
         <v>19</v>
       </c>
       <c r="J70">
-        <v>13.066016599999999</v>
+        <v>13.042828699999999</v>
       </c>
       <c r="K70">
-        <v>80.267217699999904</v>
+        <v>80.261150899999905</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B71" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C71" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D71" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E71" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
       <c r="F71" t="s">
         <v>16</v>
@@ -4482,27 +4482,27 @@
         <v>19</v>
       </c>
       <c r="J71">
-        <v>13.042828699999999</v>
+        <v>13.009577699999999</v>
       </c>
       <c r="K71">
-        <v>80.261150899999905</v>
+        <v>80.250277499999996</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B72" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C72" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D72" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E72" t="s">
-        <v>312</v>
+        <v>136</v>
       </c>
       <c r="F72" t="s">
         <v>16</v>
@@ -4517,27 +4517,27 @@
         <v>19</v>
       </c>
       <c r="J72">
-        <v>13.009577699999999</v>
+        <v>13.0323814</v>
       </c>
       <c r="K72">
-        <v>80.250277499999996</v>
+        <v>80.232834499999896</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B73" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C73" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D73" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E73" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
@@ -4552,27 +4552,27 @@
         <v>19</v>
       </c>
       <c r="J73">
-        <v>13.0323814</v>
+        <v>13.0659551</v>
       </c>
       <c r="K73">
-        <v>80.232834499999896</v>
+        <v>80.275071999999994</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B74" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C74" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D74" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>325</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
@@ -4587,27 +4587,27 @@
         <v>19</v>
       </c>
       <c r="J74">
-        <v>13.0659551</v>
+        <v>13.068490300000001</v>
       </c>
       <c r="K74">
-        <v>80.275071999999994</v>
+        <v>80.194793699999906</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B75" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C75" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D75" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="E75" t="s">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
@@ -4622,27 +4622,27 @@
         <v>19</v>
       </c>
       <c r="J75">
-        <v>13.068490300000001</v>
+        <v>12.983451799999999</v>
       </c>
       <c r="K75">
-        <v>80.194793699999906</v>
+        <v>80.2462952999999</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B76" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C76" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D76" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="E76" t="s">
-        <v>15</v>
+        <v>334</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
@@ -4657,27 +4657,27 @@
         <v>19</v>
       </c>
       <c r="J76">
-        <v>12.983451799999999</v>
+        <v>13.0638448</v>
       </c>
       <c r="K76">
-        <v>80.2462952999999</v>
+        <v>80.210179199999899</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="B77" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C77" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D77" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="E77" t="s">
-        <v>334</v>
+        <v>15</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -4692,27 +4692,27 @@
         <v>19</v>
       </c>
       <c r="J77">
-        <v>13.0638448</v>
+        <v>12.9662223</v>
       </c>
       <c r="K77">
-        <v>80.210179199999899</v>
+        <v>80.149137999999994</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B78" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C78" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D78" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="E78" t="s">
-        <v>15</v>
+        <v>343</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
@@ -4727,27 +4727,27 @@
         <v>19</v>
       </c>
       <c r="J78">
-        <v>12.9662223</v>
+        <v>12.9700638</v>
       </c>
       <c r="K78">
-        <v>80.149137999999994</v>
+        <v>80.1460521999999</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B79" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C79" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="D79" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E79" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="F79" t="s">
         <v>16</v>
@@ -4762,27 +4762,27 @@
         <v>19</v>
       </c>
       <c r="J79">
-        <v>12.9700638</v>
+        <v>13.071020000000001</v>
       </c>
       <c r="K79">
-        <v>80.1460521999999</v>
+        <v>80.211237999999895</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B80" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C80" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="D80" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="E80" t="s">
-        <v>348</v>
+        <v>15</v>
       </c>
       <c r="F80" t="s">
         <v>16</v>
@@ -4797,24 +4797,24 @@
         <v>19</v>
       </c>
       <c r="J80">
-        <v>13.071020000000001</v>
+        <v>13.0805325</v>
       </c>
       <c r="K80">
-        <v>80.211237999999895</v>
+        <v>80.269378899999893</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B81" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C81" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="D81" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -4832,24 +4832,24 @@
         <v>19</v>
       </c>
       <c r="J81">
-        <v>13.0805325</v>
+        <v>13.0460004</v>
       </c>
       <c r="K81">
-        <v>80.269378899999893</v>
+        <v>80.239401199999904</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B82" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C82" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D82" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -4867,24 +4867,24 @@
         <v>19</v>
       </c>
       <c r="J82">
-        <v>13.0460004</v>
+        <v>13.078876299999999</v>
       </c>
       <c r="K82">
-        <v>80.239401199999904</v>
+        <v>80.241307599999999</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C83" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D83" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -4902,24 +4902,24 @@
         <v>19</v>
       </c>
       <c r="J83">
-        <v>13.078876299999999</v>
+        <v>13.052080800000001</v>
       </c>
       <c r="K83">
-        <v>80.241307599999999</v>
+        <v>80.212246800000003</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B84" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C84" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D84" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -4937,27 +4937,27 @@
         <v>19</v>
       </c>
       <c r="J84">
-        <v>13.052080800000001</v>
+        <v>13.0385641</v>
       </c>
       <c r="K84">
-        <v>80.212246800000003</v>
+        <v>80.232291000000004</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B85" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C85" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D85" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="E85" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F85" t="s">
         <v>16</v>
@@ -4972,27 +4972,27 @@
         <v>19</v>
       </c>
       <c r="J85">
-        <v>13.0385641</v>
+        <v>13.037652</v>
       </c>
       <c r="K85">
-        <v>80.232291000000004</v>
+        <v>80.231413999999901</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B86" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C86" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D86" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="E86" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F86" t="s">
         <v>16</v>
@@ -5001,30 +5001,30 @@
         <v>17</v>
       </c>
       <c r="H86" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="I86" t="s">
         <v>19</v>
       </c>
       <c r="J86">
-        <v>13.037652</v>
+        <v>13.0447028</v>
       </c>
       <c r="K86">
-        <v>80.231413999999901</v>
+        <v>80.242254699999904</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="B87" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C87" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="D87" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -5036,30 +5036,30 @@
         <v>17</v>
       </c>
       <c r="H87" t="s">
-        <v>377</v>
+        <v>18</v>
       </c>
       <c r="I87" t="s">
         <v>19</v>
       </c>
       <c r="J87">
-        <v>13.0447028</v>
+        <v>13.0468963</v>
       </c>
       <c r="K87">
-        <v>80.242254699999904</v>
+        <v>80.218684599999904</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B88" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C88" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D88" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -5077,27 +5077,27 @@
         <v>19</v>
       </c>
       <c r="J88">
-        <v>13.0468963</v>
+        <v>12.959902899999999</v>
       </c>
       <c r="K88">
-        <v>80.218684599999904</v>
+        <v>80.143556199999907</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B89" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C89" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D89" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="E89" t="s">
-        <v>15</v>
+        <v>239</v>
       </c>
       <c r="F89" t="s">
         <v>16</v>
@@ -5112,27 +5112,27 @@
         <v>19</v>
       </c>
       <c r="J89">
-        <v>12.959902899999999</v>
+        <v>13.077416100000001</v>
       </c>
       <c r="K89">
-        <v>80.143556199999907</v>
+        <v>80.2625124999999</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B90" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="C90" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D90" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="E90" t="s">
-        <v>239</v>
+        <v>394</v>
       </c>
       <c r="F90" t="s">
         <v>16</v>
@@ -5147,27 +5147,27 @@
         <v>19</v>
       </c>
       <c r="J90">
-        <v>13.077416100000001</v>
+        <v>13.0951121</v>
       </c>
       <c r="K90">
-        <v>80.2625124999999</v>
+        <v>80.290615099999897</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B91" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C91" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="D91" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="E91" t="s">
-        <v>394</v>
+        <v>15</v>
       </c>
       <c r="F91" t="s">
         <v>16</v>
@@ -5182,27 +5182,27 @@
         <v>19</v>
       </c>
       <c r="J91">
-        <v>13.0951121</v>
+        <v>13.043789500000001</v>
       </c>
       <c r="K91">
-        <v>80.290615099999897</v>
+        <v>80.2711501</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B92" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C92" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D92" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="E92" t="s">
-        <v>15</v>
+        <v>403</v>
       </c>
       <c r="F92" t="s">
         <v>16</v>
@@ -5217,27 +5217,27 @@
         <v>19</v>
       </c>
       <c r="J92">
-        <v>13.043789500000001</v>
+        <v>13.0389211</v>
       </c>
       <c r="K92">
-        <v>80.2711501</v>
+        <v>80.259598199999999</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="B93" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="C93" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="D93" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="E93" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="F93" t="s">
         <v>16</v>
@@ -5252,27 +5252,27 @@
         <v>19</v>
       </c>
       <c r="J93">
-        <v>13.0389211</v>
+        <v>13.045895</v>
       </c>
       <c r="K93">
-        <v>80.259598199999999</v>
+        <v>80.247795999999994</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B94" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="C94" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D94" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="E94" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="F94" t="s">
         <v>16</v>
@@ -5287,24 +5287,24 @@
         <v>19</v>
       </c>
       <c r="J94">
-        <v>13.045895</v>
+        <v>13.064401500000001</v>
       </c>
       <c r="K94">
-        <v>80.247795999999994</v>
+        <v>80.243316300000004</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="B95" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C95" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D95" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="E95" t="s">
         <v>413</v>
@@ -5322,27 +5322,27 @@
         <v>19</v>
       </c>
       <c r="J95">
-        <v>13.064401500000001</v>
+        <v>13.064094600000001</v>
       </c>
       <c r="K95">
-        <v>80.243316300000004</v>
+        <v>80.242161600000003</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B96" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C96" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D96" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="E96" t="s">
-        <v>413</v>
+        <v>15</v>
       </c>
       <c r="F96" t="s">
         <v>16</v>
@@ -5357,27 +5357,27 @@
         <v>19</v>
       </c>
       <c r="J96">
-        <v>13.064094600000001</v>
+        <v>13.0542792</v>
       </c>
       <c r="K96">
-        <v>80.242161600000003</v>
+        <v>80.253177499999893</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B97" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D97" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="E97" t="s">
-        <v>15</v>
+        <v>403</v>
       </c>
       <c r="F97" t="s">
         <v>16</v>
@@ -5392,27 +5392,27 @@
         <v>19</v>
       </c>
       <c r="J97">
-        <v>13.0542792</v>
+        <v>13.046714100000001</v>
       </c>
       <c r="K97">
-        <v>80.253177499999893</v>
+        <v>80.266620900000007</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B98" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C98" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D98" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="E98" t="s">
-        <v>403</v>
+        <v>136</v>
       </c>
       <c r="F98" t="s">
         <v>16</v>
@@ -5427,27 +5427,27 @@
         <v>19</v>
       </c>
       <c r="J98">
-        <v>13.046714100000001</v>
+        <v>13.044298</v>
       </c>
       <c r="K98">
-        <v>80.266620900000007</v>
+        <v>80.238319699999906</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B99" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C99" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D99" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E99" t="s">
-        <v>136</v>
+        <v>434</v>
       </c>
       <c r="F99" t="s">
         <v>16</v>
@@ -5462,27 +5462,27 @@
         <v>19</v>
       </c>
       <c r="J99">
-        <v>13.044298</v>
+        <v>13.045194</v>
       </c>
       <c r="K99">
-        <v>80.238319699999906</v>
+        <v>80.189204000000004</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B100" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="C100" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D100" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="E100" t="s">
-        <v>434</v>
+        <v>15</v>
       </c>
       <c r="F100" t="s">
         <v>16</v>
@@ -5497,24 +5497,24 @@
         <v>19</v>
       </c>
       <c r="J100">
-        <v>13.045194</v>
+        <v>13.05884</v>
       </c>
       <c r="K100">
-        <v>80.189204000000004</v>
+        <v>80.263026999999894</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B101" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C101" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D101" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
@@ -5532,30 +5532,30 @@
         <v>19</v>
       </c>
       <c r="J101">
-        <v>13.05884</v>
+        <v>13.038558999999999</v>
       </c>
       <c r="K101">
-        <v>80.263026999999894</v>
+        <v>80.258137000000005</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B102" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="C102" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="D102" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="E102" t="s">
-        <v>15</v>
+        <v>447</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>448</v>
       </c>
       <c r="G102" t="s">
         <v>17</v>
@@ -5567,30 +5567,30 @@
         <v>19</v>
       </c>
       <c r="J102">
-        <v>13.038558999999999</v>
+        <v>12.844614699999999</v>
       </c>
       <c r="K102">
-        <v>80.258137000000005</v>
+        <v>80.243062699999996</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="B103" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="C103" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="D103" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="E103" t="s">
-        <v>447</v>
+        <v>136</v>
       </c>
       <c r="F103" t="s">
-        <v>448</v>
+        <v>16</v>
       </c>
       <c r="G103" t="s">
         <v>17</v>
@@ -5602,27 +5602,27 @@
         <v>19</v>
       </c>
       <c r="J103">
-        <v>12.844614699999999</v>
+        <v>13.038517300000001</v>
       </c>
       <c r="K103">
-        <v>80.243062699999996</v>
+        <v>80.239962599999998</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B104" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C104" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D104" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="E104" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F104" t="s">
         <v>16</v>
@@ -5637,24 +5637,24 @@
         <v>19</v>
       </c>
       <c r="J104">
-        <v>13.038517300000001</v>
+        <v>13.0867883</v>
       </c>
       <c r="K104">
-        <v>80.239962599999998</v>
+        <v>80.269808900000001</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B105" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C105" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="D105" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -5672,27 +5672,27 @@
         <v>19</v>
       </c>
       <c r="J105">
-        <v>13.0867883</v>
+        <v>13.067836</v>
       </c>
       <c r="K105">
-        <v>80.269808900000001</v>
+        <v>80.271991999999898</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B106" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C106" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="D106" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E106" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F106" t="s">
         <v>16</v>
@@ -5707,30 +5707,30 @@
         <v>19</v>
       </c>
       <c r="J106">
-        <v>13.067836</v>
+        <v>13.050005000000001</v>
       </c>
       <c r="K106">
-        <v>80.271991999999898</v>
+        <v>80.232989999999901</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B107" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C107" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="D107" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="E107" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="F107" t="s">
-        <v>16</v>
+        <v>469</v>
       </c>
       <c r="G107" t="s">
         <v>17</v>
@@ -5742,44 +5742,9 @@
         <v>19</v>
       </c>
       <c r="J107">
-        <v>13.050005000000001</v>
+        <v>12.764486</v>
       </c>
       <c r="K107">
-        <v>80.232989999999901</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B108" t="s">
-        <v>466</v>
-      </c>
-      <c r="C108" t="s">
-        <v>467</v>
-      </c>
-      <c r="D108" t="s">
-        <v>468</v>
-      </c>
-      <c r="E108" t="s">
-        <v>15</v>
-      </c>
-      <c r="F108" t="s">
-        <v>469</v>
-      </c>
-      <c r="G108" t="s">
-        <v>17</v>
-      </c>
-      <c r="H108" t="s">
-        <v>18</v>
-      </c>
-      <c r="I108" t="s">
-        <v>19</v>
-      </c>
-      <c r="J108">
-        <v>12.764486</v>
-      </c>
-      <c r="K108">
         <v>80.005634999999899</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added id field to locations
</commit_message>
<xml_diff>
--- a/onboarding-bootstrap/datav4.xlsx
+++ b/onboarding-bootstrap/datav4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hotels" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="datafile" localSheetId="0">hotels!$B$1:$L$66</definedName>
     <definedName name="hotels" localSheetId="0">hotels!$B$67:$L$107</definedName>
-    <definedName name="locations" localSheetId="1">locations!$A$1:$J$10</definedName>
+    <definedName name="locations" localSheetId="1">locations!$B$1:$K$10</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="524">
   <si>
     <t>placeid</t>
   </si>
@@ -1989,7 +1989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="83" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A107"/>
     </sheetView>
   </sheetViews>
@@ -6079,340 +6079,372 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>474</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>475</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>476</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>477</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>200000</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>479</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>480</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>481</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>482</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>483</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
       <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
         <v>13.198634800000001</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>77.706592799999896</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>200001</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>485</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>486</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>487</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
         <v>12.983254199999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>80.166865499999901</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>200002</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>489</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>490</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>491</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4">
         <v>12.994111999999999</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>80.170866799999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>200003</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>493</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>494</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>495</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
         <v>13.071801000000001</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>80.240476999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>200004</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>497</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>498</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>499</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>500</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>501</v>
       </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
       <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6">
         <v>22.583000200000001</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>88.3372908999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>200005</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>503</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>504</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>505</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>506</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>507</v>
       </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
       <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
         <v>17.392200500000001</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>78.467987199999897</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>200006</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>509</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>510</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>511</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>512</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>513</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
       <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8">
         <v>19.092619500000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>72.866317299999906</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>200007</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>515</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>516</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>517</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>518</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>501</v>
       </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9">
         <v>22.652042900000001</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>88.446329899999995</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>200008</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>520</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>521</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>522</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10">
         <v>13.077744900000001</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>80.261360100000005</v>
       </c>
     </row>

</xml_diff>